<commit_message>
Read execl and list values
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5267523D-3A66-4575-9375-79F3FCF19D72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A43CEC9-9F1A-4BBF-83E9-F3AE7914DFDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8835" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
     <sheet name="openings" sheetId="2" r:id="rId2"/>
     <sheet name="translations" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>36G</t>
   </si>
@@ -78,6 +79,12 @@
   </si>
   <si>
     <t>/2</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>K3</t>
   </si>
 </sst>
 </file>
@@ -409,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,50 +432,54 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="1">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C4" s="1">
         <v>46</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C5" s="1">
         <v>47</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -572,4 +583,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tests & Combine lift
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A43CEC9-9F1A-4BBF-83E9-F3AE7914DFDF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DE8673-0A99-4937-9ED7-60078ED4C973}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8835" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32850" yWindow="-1155" windowWidth="12150" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>36G</t>
   </si>
@@ -69,22 +69,46 @@
     <t>container</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>Finnish</t>
   </si>
   <si>
     <t>English</t>
   </si>
   <si>
-    <t>/2</t>
-  </si>
-  <si>
     <t>K4</t>
   </si>
   <si>
     <t>K3</t>
+  </si>
+  <si>
+    <t>Costa</t>
+  </si>
+  <si>
+    <t>K5</t>
+  </si>
+  <si>
+    <t>57G</t>
+  </si>
+  <si>
+    <t>56G</t>
+  </si>
+  <si>
+    <t>Bufetti</t>
+  </si>
+  <si>
+    <t>Putkivarasto</t>
+  </si>
+  <si>
+    <t>Kansi 3</t>
+  </si>
+  <si>
+    <t>Kansi 4</t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>OPENING</t>
   </si>
 </sst>
 </file>
@@ -418,13 +442,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="16" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
@@ -434,7 +458,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,7 +477,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -475,11 +505,13 @@
         <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -489,10 +521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76F300B-D275-41D2-B2B1-867F5B3009EE}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,9 +542,6 @@
       <c r="B1" s="1">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -521,9 +550,6 @@
       <c r="B2" s="1">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -533,7 +559,12 @@
         <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -558,10 +589,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -587,28 +618,62 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Combine message and preview
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE99BE1-6D7E-44E5-BAE2-3262CD31A1D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45429F4C-3438-4C25-83D0-02D86A9DEF0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16650" yWindow="1905" windowWidth="12150" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16650" yWindow="1905" windowWidth="12150" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
     <sheet name="openings" sheetId="2" r:id="rId2"/>
-    <sheet name="translations" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="users" sheetId="4" r:id="rId3"/>
+    <sheet name="translations" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>36G</t>
   </si>
@@ -81,24 +81,6 @@
     <t>K3</t>
   </si>
   <si>
-    <t>Costa</t>
-  </si>
-  <si>
-    <t>K5</t>
-  </si>
-  <si>
-    <t>57G</t>
-  </si>
-  <si>
-    <t>56G</t>
-  </si>
-  <si>
-    <t>Bufetti</t>
-  </si>
-  <si>
-    <t>Putkivarasto</t>
-  </si>
-  <si>
     <t>Kansi 3</t>
   </si>
   <si>
@@ -115,6 +97,9 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>Eemeli</t>
   </si>
 </sst>
 </file>
@@ -448,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -467,7 +452,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -486,7 +471,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,12 +501,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -575,12 +560,12 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -589,6 +574,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C0F865-E695-4F7D-9576-44DFD7FC5C3A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -630,69 +640,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Load & Save lifts test
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45429F4C-3438-4C25-83D0-02D86A9DEF0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786B4BA1-DBDA-4FE6-A1DE-C6C62028A728}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16650" yWindow="1905" windowWidth="12150" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
     <sheet name="openings" sheetId="2" r:id="rId2"/>
     <sheet name="users" sheetId="4" r:id="rId3"/>
-    <sheet name="translations" sheetId="3" r:id="rId4"/>
+    <sheet name="groups" sheetId="6" r:id="rId4"/>
+    <sheet name="lifts" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>36G</t>
   </si>
@@ -51,9 +52,6 @@
     <t>pääkeittiö</t>
   </si>
   <si>
-    <t>main galley</t>
-  </si>
-  <si>
     <t>036N-S</t>
   </si>
   <si>
@@ -66,15 +64,6 @@
     <t>kontti</t>
   </si>
   <si>
-    <t>container</t>
-  </si>
-  <si>
-    <t>Finnish</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
     <t>K4</t>
   </si>
   <si>
@@ -100,6 +89,24 @@
   </si>
   <si>
     <t>Eemeli</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>057G</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>Akseli</t>
   </si>
 </sst>
 </file>
@@ -431,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,10 +456,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,10 +475,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -501,12 +508,17 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +545,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1">
         <v>35</v>
@@ -541,7 +553,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>36</v>
@@ -549,23 +561,23 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -575,9 +587,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -589,7 +603,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -599,42 +618,69 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C0F865-E695-4F7D-9576-44DFD7FC5C3A}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E794B3-EFCA-427E-8DD1-88CA4959597E}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C050DD1E-C2B9-44A4-AF76-C1FBA3AA97F4}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="36.42578125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Callback keyboard response. TODO list
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786B4BA1-DBDA-4FE6-A1DE-C6C62028A728}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BABC54-DFF4-4076-B1CA-35808B76DFD5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13830" yWindow="3630" windowWidth="12150" windowHeight="11505" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
     <sheet name="openings" sheetId="2" r:id="rId2"/>
     <sheet name="users" sheetId="4" r:id="rId3"/>
     <sheet name="groups" sheetId="6" r:id="rId4"/>
-    <sheet name="lifts" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>36G</t>
   </si>
@@ -89,15 +88,6 @@
   </si>
   <si>
     <t>Eemeli</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>STATE</t>
-  </si>
-  <si>
-    <t>NOTE</t>
   </si>
   <si>
     <t>057G</t>
@@ -440,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +508,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -608,7 +598,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -621,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E794B3-EFCA-427E-8DD1-88CA4959597E}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -632,7 +622,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -642,48 +632,11 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C050DD1E-C2B9-44A4-AF76-C1FBA3AA97F4}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="36.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Lift state updating : progress, ButtonCallbackData to enum
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17BABC54-DFF4-4076-B1CA-35808B76DFD5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F71B96B-6184-415A-8F99-25AC4A03C42A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13830" yWindow="3630" windowWidth="12150" windowHeight="11505" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>36G</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>Akseli</t>
+  </si>
+  <si>
+    <t>LMG</t>
+  </si>
+  <si>
+    <t>Jukka</t>
+  </si>
+  <si>
+    <t>Juhani</t>
+  </si>
+  <si>
+    <t>Vallu</t>
+  </si>
+  <si>
+    <t>Vladimir</t>
   </si>
 </sst>
 </file>
@@ -140,12 +155,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -430,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,28 +595,47 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -609,30 +646,46 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E794B3-EFCA-427E-8DD1-88CA4959597E}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reply what shoud be typed next + Add ConversationHandler
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F71B96B-6184-415A-8F99-25AC4A03C42A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44998A12-B8A5-4866-9CBA-DA0102B94213}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
-    <sheet name="openings" sheetId="2" r:id="rId2"/>
-    <sheet name="users" sheetId="4" r:id="rId3"/>
+    <sheet name="users" sheetId="4" r:id="rId2"/>
+    <sheet name="openings" sheetId="2" r:id="rId3"/>
     <sheet name="groups" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>36G</t>
   </si>
@@ -112,6 +112,27 @@
   </si>
   <si>
     <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Nicknames ....</t>
   </si>
 </sst>
 </file>
@@ -448,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -536,6 +557,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76F300B-D275-41D2-B2B1-867F5B3009EE}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -590,57 +684,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
user_data & bot_data keys from string to enums + Ready state + Add per user signaling and linking : progress
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9709F9A5-9DBB-4D40-AD56-C2AB5A4816DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7197B375-C646-460D-9398-0C338D449C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8205" yWindow="2895" windowWidth="14790" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8835" windowWidth="16440" windowHeight="28590" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
-    <sheet name="users" sheetId="4" r:id="rId2"/>
-    <sheet name="openings" sheetId="2" r:id="rId3"/>
+    <sheet name="openings" sheetId="2" r:id="rId2"/>
+    <sheet name="users" sheetId="4" r:id="rId3"/>
     <sheet name="groups" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>36G</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Eemelioma</t>
+  </si>
+  <si>
+    <t>Log</t>
+  </si>
+  <si>
+    <t>MJ</t>
   </si>
 </sst>
 </file>
@@ -557,76 +563,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1156192071</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1389122945</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>846031989</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76F300B-D275-41D2-B2B1-867F5B3009EE}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -684,12 +620,82 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C6A986-8ABD-4C34-B1A8-960631FCCEBE}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1156192071</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1389122945</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>846031989</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E794B3-EFCA-427E-8DD1-88CA4959597E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,15 +705,21 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -715,7 +727,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -723,7 +735,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Add per user signaling and linking
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7197B375-C646-460D-9398-0C338D449C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CFDF82-1BB6-4FF3-9D6C-BA2FB854E20C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8835" windowWidth="16440" windowHeight="28590" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30765" yWindow="8130" windowWidth="9105" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
User can follow sites, Ping : progress
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/file.xlsx
+++ b/middleman-bot/middleman-bot/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\core_py\middleman-bot\middleman-bot\middleman-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CFDF82-1BB6-4FF3-9D6C-BA2FB854E20C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EC3014-2F49-41D3-97E5-197508D01576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30765" yWindow="8130" windowWidth="9105" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8715" yWindow="1485" windowWidth="9105" windowHeight="13275" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>36G</t>
   </si>
@@ -48,9 +48,6 @@
     <t>047G</t>
   </si>
   <si>
-    <t>pääkeittiö</t>
-  </si>
-  <si>
     <t>036N-S</t>
   </si>
   <si>
@@ -60,27 +57,12 @@
     <t>047G-P</t>
   </si>
   <si>
-    <t>kontti</t>
-  </si>
-  <si>
     <t>K4</t>
   </si>
   <si>
     <t>K3</t>
   </si>
   <si>
-    <t>Kansi 3</t>
-  </si>
-  <si>
-    <t>Kansi 4</t>
-  </si>
-  <si>
-    <t>SITE</t>
-  </si>
-  <si>
-    <t>OPENING</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -90,9 +72,6 @@
     <t>Eemeli</t>
   </si>
   <si>
-    <t>057G</t>
-  </si>
-  <si>
     <t>CORE</t>
   </si>
   <si>
@@ -139,6 +118,18 @@
   </si>
   <si>
     <t>MJ</t>
+  </si>
+  <si>
+    <t>046P</t>
+  </si>
+  <si>
+    <t>Pääkeittiö</t>
+  </si>
+  <si>
+    <t>Kontti</t>
+  </si>
+  <si>
+    <t>046G-S</t>
   </si>
 </sst>
 </file>
@@ -473,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,71 +480,74 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>47</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -564,10 +558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76F300B-D275-41D2-B2B1-867F5B3009EE}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,41 +572,54 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>47</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -639,25 +646,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,7 +672,7 @@
         <v>1156192071</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -673,7 +680,7 @@
         <v>1389122945</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -681,7 +688,7 @@
         <v>846031989</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -707,37 +714,37 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>